<commit_message>
Adding NetBanking and Cash Channel cases
</commit_message>
<xml_diff>
--- a/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
+++ b/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="292">
   <si>
     <t>TC_ID</t>
   </si>
@@ -822,13 +822,91 @@
   </si>
   <si>
     <t>https://airpay.co.in/ipntest/responsefromairpay.php</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_BankDetails_Active</t>
+  </si>
+  <si>
+    <t>ChannelName</t>
+  </si>
+  <si>
+    <t>NETBANKING</t>
+  </si>
+  <si>
+    <t>BankName_MAPanel</t>
+  </si>
+  <si>
+    <t>Axis-netbnk</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_BankDetails_Inactive</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_URL_Details_Active</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_URL_Details_Inactive</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_BankDetails_MinAndMax_Range_Val</t>
+  </si>
+  <si>
+    <t>MinumAmtVal</t>
+  </si>
+  <si>
+    <t>MaxAmtVal</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>200000.00</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_BankDetails_MinAndMax_Range_Val(it covers two test cases)</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_URLDetails_MinAndMax_Range_Val(it covers two test cases)</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_URLDetails_MinAndMax_Range_val</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_Merchant_BankDetails_MinAndMax_Range_Val</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_NetBanking_Merchant_URLDetails_MinAndMax_Range_val</t>
+  </si>
+  <si>
+    <t>300000.00</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_Cash_BankDetails_Inactive</t>
+  </si>
+  <si>
+    <t>ItzCash-cash</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>auth-capture</t>
+  </si>
+  <si>
+    <t>TC_MA_Panel_Cash_BankDetails_Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -931,8 +1009,64 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -975,6 +1109,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1005,7 +1151,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1049,6 +1195,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1402,10 +1565,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK148"/>
+  <dimension ref="A1:AN148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1439,13 +1602,16 @@
     <col min="28" max="30" width="34.85546875" customWidth="1"/>
     <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="34" width="37.5703125" customWidth="1"/>
-    <col min="35" max="35" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="1026" width="8.7109375" customWidth="1"/>
+    <col min="38" max="38" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="1026" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1549,7 +1715,7 @@
         <v>257</v>
       </c>
       <c r="AI1" s="21" t="s">
-        <v>20</v>
+        <v>269</v>
       </c>
       <c r="AJ1" s="21" t="s">
         <v>260</v>
@@ -1557,8 +1723,17 @@
       <c r="AK1" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+      <c r="AL1" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="AM1" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1606,7 +1781,7 @@
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
     </row>
-    <row r="3" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1651,7 +1826,7 @@
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
     </row>
-    <row r="4" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
@@ -1696,7 +1871,7 @@
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
     </row>
-    <row r="5" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>34</v>
       </c>
@@ -1741,7 +1916,7 @@
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>36</v>
       </c>
@@ -1783,7 +1958,7 @@
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
     </row>
-    <row r="7" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>38</v>
       </c>
@@ -1821,7 +1996,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
@@ -1863,7 +2038,7 @@
       <c r="AC8" s="5"/>
       <c r="AD8" s="5"/>
     </row>
-    <row r="9" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
@@ -1905,7 +2080,7 @@
       <c r="AC9" s="5"/>
       <c r="AD9" s="5"/>
     </row>
-    <row r="10" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>45</v>
       </c>
@@ -1962,7 +2137,7 @@
       <c r="AC10" s="5"/>
       <c r="AD10" s="5"/>
     </row>
-    <row r="11" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -2019,7 +2194,7 @@
       <c r="AC11" s="5"/>
       <c r="AD11" s="5"/>
     </row>
-    <row r="12" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>55</v>
       </c>
@@ -2076,7 +2251,7 @@
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
     </row>
-    <row r="13" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -2118,7 +2293,7 @@
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
     </row>
-    <row r="14" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -2175,7 +2350,7 @@
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
     </row>
-    <row r="15" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2232,7 +2407,7 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
     </row>
-    <row r="16" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
@@ -5885,87 +6060,87 @@
         <v>238</v>
       </c>
     </row>
-    <row r="94" spans="1:37" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="1:37" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="C94" t="s">
-        <v>228</v>
-      </c>
-      <c r="D94" t="s">
-        <v>23</v>
-      </c>
-      <c r="E94">
-        <v>1</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="C94" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D94" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E94" s="23">
+        <v>1</v>
+      </c>
+      <c r="F94" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="H94" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I94" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J94" t="s">
-        <v>26</v>
-      </c>
-      <c r="K94" t="s">
-        <v>27</v>
-      </c>
-      <c r="M94" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N94" t="s">
+      <c r="H94" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I94" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J94" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K94" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M94" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="N94" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="P94" s="11" t="s">
+      <c r="P94" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="S94" t="s">
+      <c r="S94" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="T94" t="s">
+      <c r="T94" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="U94" t="s">
+      <c r="U94" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="X94" s="11"/>
-      <c r="AA94" t="s">
+      <c r="X94" s="26"/>
+      <c r="AA94" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="AB94" t="s">
+      <c r="AB94" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="AC94" s="11" t="s">
+      <c r="AC94" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="AD94" t="s">
+      <c r="AD94" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="AE94" s="11" t="s">
+      <c r="AE94" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="AF94" s="22" t="s">
+      <c r="AF94" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="AG94" s="22" t="s">
+      <c r="AG94" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="AH94" s="22" t="s">
+      <c r="AH94" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="AI94" s="22" t="s">
+      <c r="AI94" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="AJ94" s="22" t="s">
+      <c r="AJ94" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="AK94" s="22" t="s">
+      <c r="AK94" s="27" t="s">
         <v>264</v>
       </c>
     </row>
@@ -5979,82 +6154,661 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>272</v>
+      </c>
+      <c r="B98" t="s">
+        <v>272</v>
+      </c>
+      <c r="C98" t="s">
+        <v>22</v>
+      </c>
+      <c r="D98" t="s">
+        <v>23</v>
+      </c>
       <c r="E98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F98" t="s">
+        <v>272</v>
+      </c>
+      <c r="H98" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I98" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J98" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K98" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L98" s="32"/>
+      <c r="M98" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N98" t="s">
+        <v>35</v>
+      </c>
+      <c r="V98" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA98" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB98" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC98" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD98" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE98" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF98" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG98" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH98" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI98" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ98" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK98" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="AL98" s="34" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="99" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>266</v>
+      </c>
+      <c r="B99" t="s">
+        <v>266</v>
+      </c>
+      <c r="C99" t="s">
+        <v>22</v>
+      </c>
+      <c r="D99" t="s">
+        <v>23</v>
+      </c>
       <c r="E99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F99" t="s">
+        <v>266</v>
+      </c>
+      <c r="H99" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I99" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J99" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K99" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L99" s="32"/>
+      <c r="M99" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N99" t="s">
+        <v>35</v>
+      </c>
+      <c r="V99" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA99" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB99" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC99" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD99" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE99" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF99" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG99" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH99" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI99" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ99" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK99" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL99" s="34" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="100" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>275</v>
+      </c>
+      <c r="B100" t="s">
+        <v>275</v>
+      </c>
+      <c r="C100" t="s">
+        <v>22</v>
+      </c>
+      <c r="D100" t="s">
+        <v>23</v>
+      </c>
       <c r="E100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F100" t="s">
+        <v>275</v>
+      </c>
+      <c r="H100" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I100" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J100" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K100" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L100" s="32"/>
+      <c r="M100" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N100" t="s">
+        <v>35</v>
+      </c>
+      <c r="V100" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA100" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB100" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC100" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD100" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE100" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF100" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG100" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH100" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI100" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ100" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK100" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="AL100" s="34"/>
+    </row>
+    <row r="101" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>274</v>
+      </c>
+      <c r="B101" t="s">
+        <v>274</v>
+      </c>
+      <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s">
+        <v>23</v>
+      </c>
       <c r="E101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F101" t="s">
+        <v>274</v>
+      </c>
+      <c r="H101" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I101" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J101" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K101" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L101" s="32"/>
+      <c r="M101" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N101" t="s">
+        <v>35</v>
+      </c>
+      <c r="V101" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA101" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB101" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC101" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD101" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE101" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF101" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG101" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH101" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI101" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ101" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK101" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL101" s="34"/>
+    </row>
+    <row r="102" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>284</v>
+      </c>
+      <c r="B102" t="s">
+        <v>281</v>
+      </c>
+      <c r="C102" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102" t="s">
+        <v>23</v>
+      </c>
       <c r="E102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F102" t="s">
+        <v>276</v>
+      </c>
+      <c r="H102" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I102" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J102" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K102" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L102" s="32"/>
+      <c r="M102" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N102" t="s">
+        <v>35</v>
+      </c>
+      <c r="V102" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA102" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB102" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC102" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD102" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE102" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF102" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG102" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH102" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI102" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ102" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK102" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL102" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM102" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="AN102" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="103" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>285</v>
+      </c>
+      <c r="B103" t="s">
+        <v>282</v>
+      </c>
+      <c r="C103" t="s">
+        <v>22</v>
+      </c>
+      <c r="D103" t="s">
+        <v>23</v>
+      </c>
       <c r="E103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F103" t="s">
+        <v>283</v>
+      </c>
+      <c r="H103" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I103" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J103" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K103" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L103" s="32"/>
+      <c r="M103" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N103" t="s">
+        <v>35</v>
+      </c>
+      <c r="V103" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA103" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB103" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC103" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD103" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE103" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF103" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG103" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH103" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI103" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ103" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK103" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL103" s="34"/>
+      <c r="AM103" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="AN103" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>287</v>
+      </c>
+      <c r="B104" t="s">
+        <v>287</v>
+      </c>
+      <c r="C104" t="s">
+        <v>228</v>
+      </c>
+      <c r="D104" t="s">
+        <v>23</v>
+      </c>
       <c r="E104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F104" t="s">
+        <v>287</v>
+      </c>
+      <c r="H104" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I104" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J104" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K104" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L104" s="32"/>
+      <c r="M104" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N104" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA104" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB104" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC104" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD104" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE104" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF104" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG104" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH104" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI104" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="AJ104" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK104" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="AL104" s="22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="105" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>291</v>
+      </c>
+      <c r="B105" t="s">
+        <v>291</v>
+      </c>
+      <c r="C105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D105" t="s">
+        <v>23</v>
+      </c>
       <c r="E105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F105" t="s">
+        <v>291</v>
+      </c>
+      <c r="H105" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I105" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J105" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K105" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L105" s="32"/>
+      <c r="M105" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N105" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA105" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB105" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC105" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD105" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE105" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF105" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG105" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="AH105" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI105" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="AJ105" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK105" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="AL105" s="22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
       <c r="E106">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
       <c r="E107">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
       <c r="E108">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
       <c r="E109">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
       <c r="E110">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
       <c r="E111">
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
       <c r="E112">
         <v>1</v>
       </c>
@@ -6337,8 +7091,16 @@
     <hyperlink ref="H91" r:id="rId94"/>
     <hyperlink ref="H93" r:id="rId95"/>
     <hyperlink ref="H94" r:id="rId96"/>
+    <hyperlink ref="H99" r:id="rId97"/>
+    <hyperlink ref="H98" r:id="rId98"/>
+    <hyperlink ref="H100" r:id="rId99"/>
+    <hyperlink ref="H101" r:id="rId100"/>
+    <hyperlink ref="H102" r:id="rId101"/>
+    <hyperlink ref="H103" r:id="rId102"/>
+    <hyperlink ref="H104" r:id="rId103"/>
+    <hyperlink ref="H105" r:id="rId104"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId97"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId105"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some more cases
</commit_message>
<xml_diff>
--- a/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
+++ b/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6562" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7010" uniqueCount="751">
   <si>
     <t>TC_ID</t>
   </si>
@@ -2063,9 +2063,6 @@
     <t>9970623774@ybx</t>
   </si>
   <si>
-    <t>TC_PP_EMI_Bank_Type_Verification_sa</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_PP_Virtual_Account_Success_transaction_testcase </t>
   </si>
   <si>
@@ -2111,70 +2108,178 @@
     <t>TC_001_CA_Panel_Tab_Header_Verify</t>
   </si>
   <si>
+    <t>5242540301806362</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_500</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_501</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_700</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_900</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_1000</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_1200</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_499</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_500</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_501</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_700</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_900</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_1000</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_1200</t>
-  </si>
-  <si>
-    <t>5242540301806362</t>
-  </si>
-  <si>
-    <t>499</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>501</t>
-  </si>
-  <si>
-    <t>900</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>1200</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_500</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_501</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_700</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_900</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_1000</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_1200</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_499</t>
-  </si>
-  <si>
-    <t>TC_PP_Moto_Transaction_Credit_Card_Successfull_Transaction_with_Surcharge_Applied_499</t>
+    <t>TC_PP_EMI_Selecting_Bank_verifying_499.99</t>
+  </si>
+  <si>
+    <t>TC_PP_EMI_Selecting_Bank_verifying_500.01</t>
+  </si>
+  <si>
+    <t>TC_PP_EMI_Selecting_Bank_verifying_501.00</t>
+  </si>
+  <si>
+    <t>TC_PP_EMI_Selecting_Bank_verifying_1000.01</t>
+  </si>
+  <si>
+    <t>TC_PP_EMI_Selecting_Bank_verifying_999.99</t>
+  </si>
+  <si>
+    <t>TC_PP_EMI_Selecting_Bank_verifying_1200</t>
+  </si>
+  <si>
+    <t>499.99</t>
+  </si>
+  <si>
+    <t>4375513511420003</t>
+  </si>
+  <si>
+    <t>ICICI</t>
+  </si>
+  <si>
+    <t>TC_PP_EMI_Selecting_Bank_verifying_NotAppliedBank</t>
+  </si>
+  <si>
+    <t>TC_PP_Wallet_Navigation_page_499.99</t>
+  </si>
+  <si>
+    <t>TC_PP_Wallet_Navigation_page_500.01</t>
+  </si>
+  <si>
+    <t>TC_PP_Wallet_Navigation_page_501.00</t>
+  </si>
+  <si>
+    <t>TC_PP_Wallet_Navigation_page_999.99</t>
+  </si>
+  <si>
+    <t>TC_PP_Wallet_Navigation_page_1000.01</t>
+  </si>
+  <si>
+    <t>TC_PP_Wallet_Navigation_page_1200</t>
+  </si>
+  <si>
+    <t>Surcharge Test cases</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_Min</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_LessThanEqTO</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_Gt</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_Inbetween</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_Oddvalue</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_MaxValue</t>
+  </si>
+  <si>
+    <t>TC_PP_Moto_Transaction_Debit_Card_Successfull_Transaction_with_Surcharge_Applied_MorethanValue</t>
+  </si>
+  <si>
+    <t>TC_PP_UPIAddress_Empty_Transaction_ErrorMessage_NewDesign_499.99</t>
+  </si>
+  <si>
+    <t>TC_PP_UPIAddress_Empty_Transaction_ErrorMessage_NewDesign_500.01</t>
+  </si>
+  <si>
+    <t>TC_PP_UPIAddress_Empty_Transaction_ErrorMessage_NewDesign_501.00</t>
+  </si>
+  <si>
+    <t>TC_PP_UPIAddress_Empty_Transaction_ErrorMessage_NewDesign_999.99</t>
+  </si>
+  <si>
+    <t>TC_PP_UPIAddress_Empty_Transaction_ErrorMessage_NewDesign_1000.01</t>
+  </si>
+  <si>
+    <t>TC_PP_UPIAddress_Empty_Transaction_ErrorMessage_NewDesign_1200.00</t>
+  </si>
+  <si>
+    <t>TC_PP_BharatOR_BarCode_img_verification_499.99</t>
+  </si>
+  <si>
+    <t>TC_PP_BharatOR_BarCode_img_verification_500.01</t>
+  </si>
+  <si>
+    <t>TC_PP_BharatOR_BarCode_img_verification_501.00</t>
+  </si>
+  <si>
+    <t>TC_PP_BharatOR_BarCode_img_verification_999.99</t>
+  </si>
+  <si>
+    <t>TC_PP_BharatOR_BarCode_img_verification_1000.00</t>
+  </si>
+  <si>
+    <t>TC_PP_BharatOR_BarCode_img_verification_1200.00</t>
+  </si>
+  <si>
+    <t>HDFC;AXIS</t>
+  </si>
+  <si>
+    <t>TC_PP_NetBanking_Specific_Bank_page_validations_499</t>
+  </si>
+  <si>
+    <t>TC_PP_NetBanking_Specific_Bank_page_validations_500.01</t>
+  </si>
+  <si>
+    <t>TC_PP_NetBanking_Specific_Bank_page_validations_501</t>
+  </si>
+  <si>
+    <t>TC_PP_NetBanking_Specific_Bank_page_validations_999.99</t>
+  </si>
+  <si>
+    <t>TC_PP_NetBanking_Specific_Bank_page_validations_1000.00</t>
+  </si>
+  <si>
+    <t>TC_PP_NetBanking_Specific_Bank_page_validations_1200.00</t>
+  </si>
+  <si>
+    <t>600.00</t>
+  </si>
+  <si>
+    <t>749.99</t>
+  </si>
+  <si>
+    <t>750.00</t>
+  </si>
+  <si>
+    <t>750.01</t>
+  </si>
+  <si>
+    <t>800.00</t>
   </si>
 </sst>
 </file>
@@ -2950,11 +3055,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BU274"/>
+  <dimension ref="A1:BU299"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4351,7 +4456,7 @@
         <v>628</v>
       </c>
       <c r="C25" t="s">
-        <v>694</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
@@ -5378,7 +5483,7 @@
         <v>631</v>
       </c>
       <c r="C46" t="s">
-        <v>694</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
         <v>23</v>
@@ -5403,9 +5508,6 @@
       </c>
       <c r="K46" t="s">
         <v>27</v>
-      </c>
-      <c r="L46" t="s">
-        <v>128</v>
       </c>
       <c r="M46" s="9" t="s">
         <v>199</v>
@@ -6634,7 +6736,7 @@
     </row>
     <row r="74" spans="1:53" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="34" t="s">
-        <v>678</v>
+        <v>186</v>
       </c>
       <c r="B74" t="s">
         <v>186</v>
@@ -6675,7 +6777,7 @@
     </row>
     <row r="75" spans="1:53" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="34" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B75" t="s">
         <v>188</v>
@@ -6725,7 +6827,7 @@
     </row>
     <row r="76" spans="1:53" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="34" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B76" t="s">
         <v>193</v>
@@ -6775,13 +6877,13 @@
     </row>
     <row r="77" spans="1:53" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="34" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B77" t="s">
         <v>630</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>694</v>
+        <v>22</v>
       </c>
       <c r="D77" t="s">
         <v>23</v>
@@ -6821,7 +6923,7 @@
     </row>
     <row r="78" spans="1:53" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="34" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B78" t="s">
         <v>196</v>
@@ -6862,7 +6964,7 @@
     </row>
     <row r="79" spans="1:53" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="34" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B79" t="s">
         <v>198</v>
@@ -6900,7 +7002,7 @@
     </row>
     <row r="80" spans="1:53" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B80" t="s">
         <v>201</v>
@@ -6938,7 +7040,7 @@
     </row>
     <row r="81" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="34" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B81" s="36" t="s">
         <v>201</v>
@@ -6976,7 +7078,7 @@
     </row>
     <row r="82" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="34" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B82" t="s">
         <v>203</v>
@@ -7014,7 +7116,7 @@
     </row>
     <row r="83" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="34" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B83" t="s">
         <v>204</v>
@@ -7052,10 +7154,10 @@
     </row>
     <row r="84" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="34" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B84" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>22</v>
@@ -7090,10 +7192,10 @@
     </row>
     <row r="85" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="34" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B85" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C85" t="s">
         <v>22</v>
@@ -7138,7 +7240,7 @@
     </row>
     <row r="86" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B86" t="s">
         <v>215</v>
@@ -7153,7 +7255,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>24</v>
@@ -7186,7 +7288,7 @@
     </row>
     <row r="87" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="34" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B87" t="s">
         <v>218</v>
@@ -7234,7 +7336,7 @@
     </row>
     <row r="88" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="34" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B88" t="s">
         <v>219</v>
@@ -7249,7 +7351,7 @@
         <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>24</v>
@@ -7282,7 +7384,7 @@
     </row>
     <row r="89" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="34" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B89" t="s">
         <v>220</v>
@@ -7297,7 +7399,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H89" s="6" t="s">
         <v>24</v>
@@ -7330,7 +7432,7 @@
     </row>
     <row r="90" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="34" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B90" t="s">
         <v>220</v>
@@ -7381,7 +7483,7 @@
         <v>222</v>
       </c>
       <c r="B91" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C91" t="s">
         <v>22</v>
@@ -7401,10 +7503,10 @@
     </row>
     <row r="93" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="34" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B93" s="36" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C93" t="s">
         <v>22</v>
@@ -7416,7 +7518,7 @@
         <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H93" s="6" t="s">
         <v>24</v>
@@ -7434,7 +7536,7 @@
         <v>33</v>
       </c>
       <c r="N93" s="17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="Y93" s="9" t="s">
         <v>210</v>
@@ -7447,10 +7549,10 @@
     </row>
     <row r="94" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="34" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B94" s="36" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C94" t="s">
         <v>22</v>
@@ -7462,7 +7564,7 @@
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H94" s="6" t="s">
         <v>24</v>
@@ -7480,7 +7582,7 @@
         <v>33</v>
       </c>
       <c r="N94" s="17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="Y94" s="9" t="s">
         <v>210</v>
@@ -7493,10 +7595,10 @@
     </row>
     <row r="95" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="34" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B95" s="36" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C95" t="s">
         <v>22</v>
@@ -7508,7 +7610,7 @@
         <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>24</v>
@@ -7526,7 +7628,7 @@
         <v>33</v>
       </c>
       <c r="N95" s="17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="Y95" s="9" t="s">
         <v>210</v>
@@ -7539,10 +7641,10 @@
     </row>
     <row r="96" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="34" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B96" s="36" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C96" t="s">
         <v>22</v>
@@ -7554,7 +7656,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>24</v>
@@ -7572,7 +7674,7 @@
         <v>33</v>
       </c>
       <c r="N96" s="17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="Y96" s="9" t="s">
         <v>210</v>
@@ -15784,7 +15886,7 @@
         <v>1</v>
       </c>
       <c r="AA238" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="239" spans="1:46" x14ac:dyDescent="0.2">
@@ -15794,39 +15896,39 @@
     </row>
     <row r="240" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>690</v>
+      </c>
+      <c r="B240" t="s">
+        <v>690</v>
+      </c>
+      <c r="C240" t="s">
+        <v>22</v>
+      </c>
+      <c r="D240" t="s">
+        <v>23</v>
+      </c>
+      <c r="E240">
+        <v>1</v>
+      </c>
+      <c r="F240" t="s">
+        <v>690</v>
+      </c>
+      <c r="AA240" t="s">
+        <v>689</v>
+      </c>
+      <c r="AC240" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD240" t="s">
         <v>691</v>
-      </c>
-      <c r="B240" t="s">
-        <v>691</v>
-      </c>
-      <c r="C240" t="s">
-        <v>22</v>
-      </c>
-      <c r="D240" t="s">
-        <v>23</v>
-      </c>
-      <c r="E240">
-        <v>1</v>
-      </c>
-      <c r="F240" t="s">
-        <v>691</v>
-      </c>
-      <c r="AA240" t="s">
-        <v>690</v>
-      </c>
-      <c r="AC240" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD240" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="241" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B241" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C241" t="s">
         <v>22</v>
@@ -15838,207 +15940,45 @@
         <v>1</v>
       </c>
       <c r="F241" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="L241" s="37"/>
       <c r="AA241" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="AC241" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AD241" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="242" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="E242">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>714</v>
-      </c>
-      <c r="C243" t="s">
-        <v>22</v>
-      </c>
-      <c r="D243" t="s">
-        <v>23</v>
-      </c>
-      <c r="E243">
-        <v>1</v>
-      </c>
-      <c r="F243" t="s">
-        <v>429</v>
-      </c>
-      <c r="H243" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I243" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J243" t="s">
-        <v>145</v>
-      </c>
-      <c r="K243" t="s">
-        <v>146</v>
-      </c>
-      <c r="L243" t="s">
-        <v>622</v>
-      </c>
-      <c r="M243" s="9" t="s">
-        <v>702</v>
-      </c>
-      <c r="N243" t="s">
-        <v>54</v>
-      </c>
-      <c r="P243" s="9" t="s">
-        <v>701</v>
-      </c>
-      <c r="T243" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="U243" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB243" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="AC243" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="AD243" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="AE243" s="22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="244" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>695</v>
-      </c>
-      <c r="C244" t="s">
-        <v>22</v>
-      </c>
-      <c r="D244" t="s">
-        <v>23</v>
-      </c>
-      <c r="E244">
-        <v>1</v>
-      </c>
-      <c r="F244" t="s">
-        <v>429</v>
-      </c>
-      <c r="H244" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I244" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J244" t="s">
-        <v>145</v>
-      </c>
-      <c r="K244" t="s">
-        <v>146</v>
-      </c>
-      <c r="L244" t="s">
-        <v>622</v>
-      </c>
-      <c r="M244" s="9" t="s">
-        <v>703</v>
-      </c>
-      <c r="N244" t="s">
-        <v>54</v>
-      </c>
-      <c r="P244" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="T244" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="U244" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB244" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="AC244" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="AD244" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="AE244" s="22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="245" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>696</v>
-      </c>
-      <c r="C245" t="s">
-        <v>22</v>
-      </c>
-      <c r="D245" t="s">
-        <v>23</v>
-      </c>
+      <c r="L242" s="37"/>
+      <c r="AC242" s="9"/>
+    </row>
+    <row r="243" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="L243" s="37"/>
+      <c r="AC243" s="9"/>
+    </row>
+    <row r="244" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A244" s="29" t="s">
+        <v>719</v>
+      </c>
+      <c r="L244" s="37"/>
+      <c r="AC244" s="9"/>
+    </row>
+    <row r="245" spans="1:31" x14ac:dyDescent="0.2">
       <c r="E245">
         <v>1</v>
-      </c>
-      <c r="F245" t="s">
-        <v>429</v>
-      </c>
-      <c r="H245" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I245" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J245" t="s">
-        <v>145</v>
-      </c>
-      <c r="K245" t="s">
-        <v>146</v>
-      </c>
-      <c r="L245" t="s">
-        <v>622</v>
-      </c>
-      <c r="M245" s="9" t="s">
-        <v>704</v>
-      </c>
-      <c r="N245" t="s">
-        <v>54</v>
-      </c>
-      <c r="P245" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="T245" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="U245" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB245" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="AC245" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="AD245" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="AE245" s="22" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="246" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>697</v>
+        <v>720</v>
       </c>
       <c r="C246" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D246" t="s">
         <v>23</v>
@@ -16065,14 +16005,15 @@
         <v>622</v>
       </c>
       <c r="M246" s="9" t="s">
-        <v>379</v>
+        <v>709</v>
       </c>
       <c r="N246" t="s">
         <v>54</v>
       </c>
       <c r="P246" s="9" t="s">
-        <v>623</v>
-      </c>
+        <v>693</v>
+      </c>
+      <c r="Q246" s="9"/>
       <c r="T246" s="9" t="s">
         <v>148</v>
       </c>
@@ -16094,10 +16035,10 @@
     </row>
     <row r="247" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>698</v>
+        <v>721</v>
       </c>
       <c r="C247" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D247" t="s">
         <v>23</v>
@@ -16124,13 +16065,13 @@
         <v>622</v>
       </c>
       <c r="M247" s="9" t="s">
-        <v>705</v>
+        <v>746</v>
       </c>
       <c r="N247" t="s">
         <v>54</v>
       </c>
       <c r="P247" s="9" t="s">
-        <v>623</v>
+        <v>693</v>
       </c>
       <c r="T247" s="9" t="s">
         <v>148</v>
@@ -16153,10 +16094,10 @@
     </row>
     <row r="248" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>699</v>
+        <v>722</v>
       </c>
       <c r="C248" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D248" t="s">
         <v>23</v>
@@ -16183,13 +16124,13 @@
         <v>622</v>
       </c>
       <c r="M248" s="9" t="s">
-        <v>706</v>
+        <v>747</v>
       </c>
       <c r="N248" t="s">
         <v>54</v>
       </c>
       <c r="P248" s="9" t="s">
-        <v>623</v>
+        <v>693</v>
       </c>
       <c r="T248" s="9" t="s">
         <v>148</v>
@@ -16212,10 +16153,10 @@
     </row>
     <row r="249" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>700</v>
+        <v>723</v>
       </c>
       <c r="C249" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D249" t="s">
         <v>23</v>
@@ -16242,13 +16183,13 @@
         <v>622</v>
       </c>
       <c r="M249" s="9" t="s">
-        <v>707</v>
+        <v>748</v>
       </c>
       <c r="N249" t="s">
         <v>54</v>
       </c>
       <c r="P249" s="9" t="s">
-        <v>623</v>
+        <v>693</v>
       </c>
       <c r="T249" s="9" t="s">
         <v>148</v>
@@ -16269,17 +16210,71 @@
         <v>231</v>
       </c>
     </row>
-    <row r="250" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>724</v>
+      </c>
+      <c r="C250" t="s">
+        <v>702</v>
+      </c>
+      <c r="D250" t="s">
+        <v>23</v>
+      </c>
       <c r="E250">
         <v>1</v>
+      </c>
+      <c r="F250" t="s">
+        <v>429</v>
+      </c>
+      <c r="H250" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I250" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J250" t="s">
+        <v>145</v>
+      </c>
+      <c r="K250" t="s">
+        <v>146</v>
+      </c>
+      <c r="L250" t="s">
+        <v>622</v>
+      </c>
+      <c r="M250" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="N250" t="s">
+        <v>54</v>
+      </c>
+      <c r="P250" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="T250" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U250" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB250" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC250" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD250" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE250" s="22" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="251" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>715</v>
+        <v>725</v>
       </c>
       <c r="C251" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D251" t="s">
         <v>23</v>
@@ -16288,7 +16283,7 @@
         <v>1</v>
       </c>
       <c r="F251" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="H251" s="23" t="s">
         <v>24</v>
@@ -16303,16 +16298,16 @@
         <v>146</v>
       </c>
       <c r="L251" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="M251" s="9" t="s">
-        <v>702</v>
+        <v>750</v>
       </c>
       <c r="N251" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="P251" s="9" t="s">
-        <v>147</v>
+        <v>693</v>
       </c>
       <c r="T251" s="9" t="s">
         <v>148</v>
@@ -16335,10 +16330,10 @@
     </row>
     <row r="252" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>708</v>
+        <v>726</v>
       </c>
       <c r="C252" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D252" t="s">
         <v>23</v>
@@ -16347,7 +16342,7 @@
         <v>1</v>
       </c>
       <c r="F252" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="H252" s="23" t="s">
         <v>24</v>
@@ -16362,16 +16357,16 @@
         <v>146</v>
       </c>
       <c r="L252" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="M252" s="9" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
       <c r="N252" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="P252" s="9" t="s">
-        <v>147</v>
+        <v>693</v>
       </c>
       <c r="T252" s="9" t="s">
         <v>148</v>
@@ -16392,71 +16387,17 @@
         <v>231</v>
       </c>
     </row>
-    <row r="253" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>709</v>
-      </c>
-      <c r="C253" t="s">
-        <v>22</v>
-      </c>
-      <c r="D253" t="s">
-        <v>23</v>
-      </c>
+    <row r="253" spans="1:31" x14ac:dyDescent="0.2">
       <c r="E253">
         <v>1</v>
-      </c>
-      <c r="F253" t="s">
-        <v>426</v>
-      </c>
-      <c r="H253" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I253" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J253" t="s">
-        <v>145</v>
-      </c>
-      <c r="K253" t="s">
-        <v>146</v>
-      </c>
-      <c r="L253" t="s">
-        <v>619</v>
-      </c>
-      <c r="M253" s="9" t="s">
-        <v>704</v>
-      </c>
-      <c r="N253" t="s">
-        <v>46</v>
-      </c>
-      <c r="P253" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="T253" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="U253" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB253" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="AC253" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="AD253" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="AE253" s="22" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="254" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="C254" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D254" t="s">
         <v>23</v>
@@ -16483,13 +16424,13 @@
         <v>619</v>
       </c>
       <c r="M254" s="9" t="s">
-        <v>379</v>
+        <v>709</v>
       </c>
       <c r="N254" t="s">
         <v>46</v>
       </c>
       <c r="P254" s="9" t="s">
-        <v>147</v>
+        <v>710</v>
       </c>
       <c r="T254" s="9" t="s">
         <v>148</v>
@@ -16512,10 +16453,10 @@
     </row>
     <row r="255" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>711</v>
+        <v>695</v>
       </c>
       <c r="C255" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D255" t="s">
         <v>23</v>
@@ -16542,13 +16483,13 @@
         <v>619</v>
       </c>
       <c r="M255" s="9" t="s">
-        <v>705</v>
+        <v>746</v>
       </c>
       <c r="N255" t="s">
         <v>46</v>
       </c>
       <c r="P255" s="9" t="s">
-        <v>147</v>
+        <v>710</v>
       </c>
       <c r="T255" s="9" t="s">
         <v>148</v>
@@ -16571,10 +16512,10 @@
     </row>
     <row r="256" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>712</v>
+        <v>696</v>
       </c>
       <c r="C256" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D256" t="s">
         <v>23</v>
@@ -16601,13 +16542,13 @@
         <v>619</v>
       </c>
       <c r="M256" s="9" t="s">
-        <v>706</v>
+        <v>747</v>
       </c>
       <c r="N256" t="s">
         <v>46</v>
       </c>
       <c r="P256" s="9" t="s">
-        <v>147</v>
+        <v>710</v>
       </c>
       <c r="T256" s="9" t="s">
         <v>148</v>
@@ -16630,10 +16571,10 @@
     </row>
     <row r="257" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>713</v>
+        <v>697</v>
       </c>
       <c r="C257" t="s">
-        <v>22</v>
+        <v>702</v>
       </c>
       <c r="D257" t="s">
         <v>23</v>
@@ -16660,13 +16601,13 @@
         <v>619</v>
       </c>
       <c r="M257" s="9" t="s">
-        <v>707</v>
+        <v>748</v>
       </c>
       <c r="N257" t="s">
         <v>46</v>
       </c>
       <c r="P257" s="9" t="s">
-        <v>147</v>
+        <v>710</v>
       </c>
       <c r="T257" s="9" t="s">
         <v>148</v>
@@ -16687,19 +16628,181 @@
         <v>231</v>
       </c>
     </row>
-    <row r="258" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>698</v>
+      </c>
+      <c r="C258" t="s">
+        <v>702</v>
+      </c>
+      <c r="D258" t="s">
+        <v>23</v>
+      </c>
       <c r="E258">
         <v>1</v>
       </c>
-    </row>
-    <row r="259" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F258" t="s">
+        <v>426</v>
+      </c>
+      <c r="H258" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I258" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J258" t="s">
+        <v>145</v>
+      </c>
+      <c r="K258" t="s">
+        <v>146</v>
+      </c>
+      <c r="L258" t="s">
+        <v>619</v>
+      </c>
+      <c r="M258" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="N258" t="s">
+        <v>46</v>
+      </c>
+      <c r="P258" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T258" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U258" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB258" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC258" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD258" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE258" s="22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="259" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>699</v>
+      </c>
+      <c r="C259" t="s">
+        <v>702</v>
+      </c>
+      <c r="D259" t="s">
+        <v>23</v>
+      </c>
       <c r="E259">
         <v>1</v>
       </c>
-    </row>
-    <row r="260" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F259" t="s">
+        <v>426</v>
+      </c>
+      <c r="H259" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I259" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J259" t="s">
+        <v>145</v>
+      </c>
+      <c r="K259" t="s">
+        <v>146</v>
+      </c>
+      <c r="L259" t="s">
+        <v>619</v>
+      </c>
+      <c r="M259" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="N259" t="s">
+        <v>46</v>
+      </c>
+      <c r="P259" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T259" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U259" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB259" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC259" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD259" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE259" s="22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="260" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>700</v>
+      </c>
+      <c r="C260" t="s">
+        <v>702</v>
+      </c>
+      <c r="D260" t="s">
+        <v>23</v>
+      </c>
       <c r="E260">
         <v>1</v>
+      </c>
+      <c r="F260" t="s">
+        <v>426</v>
+      </c>
+      <c r="H260" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I260" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J260" t="s">
+        <v>145</v>
+      </c>
+      <c r="K260" t="s">
+        <v>146</v>
+      </c>
+      <c r="L260" t="s">
+        <v>619</v>
+      </c>
+      <c r="M260" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="N260" t="s">
+        <v>46</v>
+      </c>
+      <c r="P260" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T260" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U260" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB260" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC260" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD260" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE260" s="22" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="261" spans="1:31" x14ac:dyDescent="0.2">
@@ -16712,39 +16815,375 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A263" s="34" t="s">
+        <v>703</v>
+      </c>
+      <c r="B263" t="s">
+        <v>630</v>
+      </c>
+      <c r="C263" t="s">
+        <v>702</v>
+      </c>
+      <c r="D263" t="s">
+        <v>23</v>
+      </c>
       <c r="E263">
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F263" t="s">
+        <v>192</v>
+      </c>
+      <c r="H263" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I263" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J263" t="s">
+        <v>26</v>
+      </c>
+      <c r="K263" t="s">
+        <v>27</v>
+      </c>
+      <c r="M263" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="N263" t="s">
+        <v>76</v>
+      </c>
+      <c r="P263" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q263" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T263" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U263" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V263" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="264" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A264" s="34" t="s">
+        <v>704</v>
+      </c>
+      <c r="B264" t="s">
+        <v>630</v>
+      </c>
+      <c r="C264" t="s">
+        <v>702</v>
+      </c>
+      <c r="D264" t="s">
+        <v>23</v>
+      </c>
       <c r="E264">
         <v>1</v>
       </c>
-    </row>
-    <row r="265" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F264" t="s">
+        <v>192</v>
+      </c>
+      <c r="H264" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I264" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J264" t="s">
+        <v>26</v>
+      </c>
+      <c r="K264" t="s">
+        <v>27</v>
+      </c>
+      <c r="M264" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="N264" t="s">
+        <v>76</v>
+      </c>
+      <c r="P264" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q264" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T264" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U264" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V264" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="265" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A265" s="34" t="s">
+        <v>705</v>
+      </c>
+      <c r="B265" t="s">
+        <v>630</v>
+      </c>
+      <c r="C265" t="s">
+        <v>702</v>
+      </c>
+      <c r="D265" t="s">
+        <v>23</v>
+      </c>
       <c r="E265">
         <v>1</v>
       </c>
-    </row>
-    <row r="266" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F265" t="s">
+        <v>192</v>
+      </c>
+      <c r="H265" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I265" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J265" t="s">
+        <v>26</v>
+      </c>
+      <c r="K265" t="s">
+        <v>27</v>
+      </c>
+      <c r="M265" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="N265" t="s">
+        <v>76</v>
+      </c>
+      <c r="P265" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q265" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T265" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U265" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V265" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="266" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A266" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="B266" t="s">
+        <v>630</v>
+      </c>
+      <c r="C266" t="s">
+        <v>702</v>
+      </c>
+      <c r="D266" t="s">
+        <v>23</v>
+      </c>
       <c r="E266">
         <v>1</v>
       </c>
-    </row>
-    <row r="267" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F266" t="s">
+        <v>192</v>
+      </c>
+      <c r="H266" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I266" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J266" t="s">
+        <v>26</v>
+      </c>
+      <c r="K266" t="s">
+        <v>27</v>
+      </c>
+      <c r="M266" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="N266" t="s">
+        <v>76</v>
+      </c>
+      <c r="P266" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q266" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T266" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U266" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V266" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="267" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A267" s="34" t="s">
+        <v>706</v>
+      </c>
+      <c r="B267" t="s">
+        <v>630</v>
+      </c>
+      <c r="C267" t="s">
+        <v>702</v>
+      </c>
+      <c r="D267" t="s">
+        <v>23</v>
+      </c>
       <c r="E267">
         <v>1</v>
       </c>
-    </row>
-    <row r="268" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F267" t="s">
+        <v>192</v>
+      </c>
+      <c r="H267" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I267" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J267" t="s">
+        <v>26</v>
+      </c>
+      <c r="K267" t="s">
+        <v>27</v>
+      </c>
+      <c r="M267" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="N267" t="s">
+        <v>76</v>
+      </c>
+      <c r="P267" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q267" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T267" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U267" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V267" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="268" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A268" s="34" t="s">
+        <v>708</v>
+      </c>
+      <c r="B268" t="s">
+        <v>630</v>
+      </c>
+      <c r="C268" t="s">
+        <v>702</v>
+      </c>
+      <c r="D268" t="s">
+        <v>23</v>
+      </c>
       <c r="E268">
         <v>1</v>
       </c>
-    </row>
-    <row r="269" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F268" t="s">
+        <v>192</v>
+      </c>
+      <c r="H268" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I268" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J268" t="s">
+        <v>26</v>
+      </c>
+      <c r="K268" t="s">
+        <v>27</v>
+      </c>
+      <c r="M268" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="N268" t="s">
+        <v>76</v>
+      </c>
+      <c r="P268" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q268" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T268" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U268" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V268" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="269" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A269" s="34" t="s">
+        <v>712</v>
+      </c>
+      <c r="B269" t="s">
+        <v>630</v>
+      </c>
+      <c r="C269" t="s">
+        <v>702</v>
+      </c>
+      <c r="D269" t="s">
+        <v>23</v>
+      </c>
       <c r="E269">
         <v>1</v>
+      </c>
+      <c r="F269" t="s">
+        <v>192</v>
+      </c>
+      <c r="H269" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I269" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J269" t="s">
+        <v>26</v>
+      </c>
+      <c r="K269" t="s">
+        <v>27</v>
+      </c>
+      <c r="M269" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="N269" t="s">
+        <v>76</v>
+      </c>
+      <c r="P269" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q269" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="T269" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="U269" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V269" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="270" spans="1:31" x14ac:dyDescent="0.2">
@@ -16752,24 +17191,1195 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A271" s="29" t="s">
+        <v>713</v>
+      </c>
+      <c r="B271" t="s">
+        <v>631</v>
+      </c>
+      <c r="C271" t="s">
+        <v>702</v>
+      </c>
+      <c r="D271" t="s">
+        <v>23</v>
+      </c>
       <c r="E271">
         <v>1</v>
       </c>
-    </row>
-    <row r="272" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="F271" t="s">
+        <v>126</v>
+      </c>
+      <c r="G271" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H271" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I271" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J271" t="s">
+        <v>26</v>
+      </c>
+      <c r="K271" t="s">
+        <v>27</v>
+      </c>
+      <c r="M271" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="N271" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA271" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB271" s="5"/>
+      <c r="AC271" s="5"/>
+      <c r="AD271" s="5"/>
+    </row>
+    <row r="272" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A272" s="29" t="s">
+        <v>714</v>
+      </c>
+      <c r="B272" t="s">
+        <v>631</v>
+      </c>
+      <c r="C272" t="s">
+        <v>702</v>
+      </c>
+      <c r="D272" t="s">
+        <v>23</v>
+      </c>
       <c r="E272">
         <v>1</v>
       </c>
-    </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F272" t="s">
+        <v>126</v>
+      </c>
+      <c r="G272" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H272" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I272" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J272" t="s">
+        <v>26</v>
+      </c>
+      <c r="K272" t="s">
+        <v>27</v>
+      </c>
+      <c r="M272" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="N272" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA272" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB272" s="5"/>
+      <c r="AC272" s="5"/>
+      <c r="AD272" s="5"/>
+    </row>
+    <row r="273" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A273" s="29" t="s">
+        <v>715</v>
+      </c>
+      <c r="B273" t="s">
+        <v>631</v>
+      </c>
+      <c r="C273" t="s">
+        <v>702</v>
+      </c>
+      <c r="D273" t="s">
+        <v>23</v>
+      </c>
       <c r="E273">
         <v>1</v>
       </c>
-    </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="F273" t="s">
+        <v>126</v>
+      </c>
+      <c r="G273" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H273" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I273" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J273" t="s">
+        <v>26</v>
+      </c>
+      <c r="K273" t="s">
+        <v>27</v>
+      </c>
+      <c r="M273" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="N273" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA273" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB273" s="5"/>
+      <c r="AC273" s="5"/>
+      <c r="AD273" s="5"/>
+    </row>
+    <row r="274" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A274" s="29" t="s">
+        <v>716</v>
+      </c>
+      <c r="B274" t="s">
+        <v>631</v>
+      </c>
+      <c r="C274" t="s">
+        <v>702</v>
+      </c>
+      <c r="D274" t="s">
+        <v>23</v>
+      </c>
       <c r="E274">
         <v>1</v>
+      </c>
+      <c r="F274" t="s">
+        <v>126</v>
+      </c>
+      <c r="G274" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H274" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I274" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J274" t="s">
+        <v>26</v>
+      </c>
+      <c r="K274" t="s">
+        <v>27</v>
+      </c>
+      <c r="M274" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="N274" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA274" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB274" s="5"/>
+      <c r="AC274" s="5"/>
+      <c r="AD274" s="5"/>
+    </row>
+    <row r="275" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A275" s="29" t="s">
+        <v>717</v>
+      </c>
+      <c r="B275" t="s">
+        <v>631</v>
+      </c>
+      <c r="C275" t="s">
+        <v>702</v>
+      </c>
+      <c r="D275" t="s">
+        <v>23</v>
+      </c>
+      <c r="E275">
+        <v>1</v>
+      </c>
+      <c r="F275" t="s">
+        <v>126</v>
+      </c>
+      <c r="G275" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H275" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I275" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J275" t="s">
+        <v>26</v>
+      </c>
+      <c r="K275" t="s">
+        <v>27</v>
+      </c>
+      <c r="M275" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="N275" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA275" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB275" s="5"/>
+      <c r="AC275" s="5"/>
+      <c r="AD275" s="5"/>
+    </row>
+    <row r="276" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A276" s="29" t="s">
+        <v>718</v>
+      </c>
+      <c r="B276" t="s">
+        <v>631</v>
+      </c>
+      <c r="C276" t="s">
+        <v>702</v>
+      </c>
+      <c r="D276" t="s">
+        <v>23</v>
+      </c>
+      <c r="E276">
+        <v>1</v>
+      </c>
+      <c r="F276" t="s">
+        <v>126</v>
+      </c>
+      <c r="G276" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H276" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I276" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J276" t="s">
+        <v>26</v>
+      </c>
+      <c r="K276" t="s">
+        <v>27</v>
+      </c>
+      <c r="M276" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="N276" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA276" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB276" s="5"/>
+      <c r="AC276" s="5"/>
+      <c r="AD276" s="5"/>
+    </row>
+    <row r="277" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A277" s="29"/>
+      <c r="C277" s="15"/>
+      <c r="G277" s="5"/>
+      <c r="H277" s="6"/>
+      <c r="I277" s="7"/>
+      <c r="M277" s="9"/>
+      <c r="AB277" s="5"/>
+      <c r="AC277" s="5"/>
+      <c r="AD277" s="5"/>
+    </row>
+    <row r="278" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A278" s="29"/>
+      <c r="C278" s="15"/>
+      <c r="G278" s="5"/>
+      <c r="H278" s="6"/>
+      <c r="I278" s="7"/>
+      <c r="M278" s="9"/>
+      <c r="AB278" s="5"/>
+      <c r="AC278" s="5"/>
+      <c r="AD278" s="5"/>
+    </row>
+    <row r="279" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="E279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A280" s="34" t="s">
+        <v>727</v>
+      </c>
+      <c r="B280" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="C280" t="s">
+        <v>702</v>
+      </c>
+      <c r="D280" t="s">
+        <v>23</v>
+      </c>
+      <c r="E280">
+        <v>1</v>
+      </c>
+      <c r="F280" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="H280" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I280" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J280" t="s">
+        <v>26</v>
+      </c>
+      <c r="K280" t="s">
+        <v>27</v>
+      </c>
+      <c r="M280" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="N280" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y280" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z280" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW280" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX280" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY280" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ280" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="BA280" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="281" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A281" s="34" t="s">
+        <v>728</v>
+      </c>
+      <c r="B281" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="C281" t="s">
+        <v>702</v>
+      </c>
+      <c r="D281" t="s">
+        <v>23</v>
+      </c>
+      <c r="E281">
+        <v>1</v>
+      </c>
+      <c r="F281" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="H281" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I281" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J281" t="s">
+        <v>26</v>
+      </c>
+      <c r="K281" t="s">
+        <v>27</v>
+      </c>
+      <c r="M281" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="N281" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y281" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z281" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW281" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX281" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY281" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ281" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="BA281" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="282" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A282" s="34" t="s">
+        <v>729</v>
+      </c>
+      <c r="B282" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="C282" t="s">
+        <v>702</v>
+      </c>
+      <c r="D282" t="s">
+        <v>23</v>
+      </c>
+      <c r="E282">
+        <v>1</v>
+      </c>
+      <c r="F282" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="H282" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I282" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J282" t="s">
+        <v>26</v>
+      </c>
+      <c r="K282" t="s">
+        <v>27</v>
+      </c>
+      <c r="M282" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="N282" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y282" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z282" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW282" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX282" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY282" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ282" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="BA282" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="283" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A283" s="34" t="s">
+        <v>730</v>
+      </c>
+      <c r="B283" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="C283" t="s">
+        <v>702</v>
+      </c>
+      <c r="D283" t="s">
+        <v>23</v>
+      </c>
+      <c r="E283">
+        <v>1</v>
+      </c>
+      <c r="F283" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="H283" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I283" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J283" t="s">
+        <v>26</v>
+      </c>
+      <c r="K283" t="s">
+        <v>27</v>
+      </c>
+      <c r="M283" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="N283" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y283" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z283" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW283" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX283" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY283" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ283" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="BA283" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="284" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A284" s="34" t="s">
+        <v>731</v>
+      </c>
+      <c r="B284" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="C284" t="s">
+        <v>702</v>
+      </c>
+      <c r="D284" t="s">
+        <v>23</v>
+      </c>
+      <c r="E284">
+        <v>1</v>
+      </c>
+      <c r="F284" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="H284" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I284" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J284" t="s">
+        <v>26</v>
+      </c>
+      <c r="K284" t="s">
+        <v>27</v>
+      </c>
+      <c r="M284" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="N284" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y284" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z284" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW284" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX284" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY284" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ284" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="BA284" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="285" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A285" s="34" t="s">
+        <v>732</v>
+      </c>
+      <c r="B285" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="C285" t="s">
+        <v>702</v>
+      </c>
+      <c r="D285" t="s">
+        <v>23</v>
+      </c>
+      <c r="E285">
+        <v>1</v>
+      </c>
+      <c r="F285" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="H285" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I285" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J285" t="s">
+        <v>26</v>
+      </c>
+      <c r="K285" t="s">
+        <v>27</v>
+      </c>
+      <c r="M285" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="N285" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y285" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z285" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="AW285" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX285" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY285" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AZ285" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="BA285" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="287" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A287" s="34" t="s">
+        <v>733</v>
+      </c>
+      <c r="B287" t="s">
+        <v>198</v>
+      </c>
+      <c r="C287" t="s">
+        <v>702</v>
+      </c>
+      <c r="D287" t="s">
+        <v>23</v>
+      </c>
+      <c r="E287">
+        <v>1</v>
+      </c>
+      <c r="F287" t="s">
+        <v>198</v>
+      </c>
+      <c r="H287" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I287" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J287" t="s">
+        <v>26</v>
+      </c>
+      <c r="K287" t="s">
+        <v>27</v>
+      </c>
+      <c r="M287" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="N287" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="288" spans="1:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="A288" s="34" t="s">
+        <v>734</v>
+      </c>
+      <c r="B288" t="s">
+        <v>198</v>
+      </c>
+      <c r="C288" t="s">
+        <v>702</v>
+      </c>
+      <c r="D288" t="s">
+        <v>23</v>
+      </c>
+      <c r="E288">
+        <v>1</v>
+      </c>
+      <c r="F288" t="s">
+        <v>198</v>
+      </c>
+      <c r="H288" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I288" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J288" t="s">
+        <v>26</v>
+      </c>
+      <c r="K288" t="s">
+        <v>27</v>
+      </c>
+      <c r="M288" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="N288" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="289" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A289" s="34" t="s">
+        <v>735</v>
+      </c>
+      <c r="B289" t="s">
+        <v>198</v>
+      </c>
+      <c r="C289" t="s">
+        <v>702</v>
+      </c>
+      <c r="D289" t="s">
+        <v>23</v>
+      </c>
+      <c r="E289">
+        <v>1</v>
+      </c>
+      <c r="F289" t="s">
+        <v>198</v>
+      </c>
+      <c r="H289" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I289" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J289" t="s">
+        <v>26</v>
+      </c>
+      <c r="K289" t="s">
+        <v>27</v>
+      </c>
+      <c r="M289" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="N289" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="290" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A290" s="34" t="s">
+        <v>736</v>
+      </c>
+      <c r="B290" t="s">
+        <v>198</v>
+      </c>
+      <c r="C290" t="s">
+        <v>702</v>
+      </c>
+      <c r="D290" t="s">
+        <v>23</v>
+      </c>
+      <c r="E290">
+        <v>1</v>
+      </c>
+      <c r="F290" t="s">
+        <v>198</v>
+      </c>
+      <c r="H290" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I290" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J290" t="s">
+        <v>26</v>
+      </c>
+      <c r="K290" t="s">
+        <v>27</v>
+      </c>
+      <c r="M290" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="N290" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="291" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A291" s="34" t="s">
+        <v>737</v>
+      </c>
+      <c r="B291" t="s">
+        <v>198</v>
+      </c>
+      <c r="C291" t="s">
+        <v>702</v>
+      </c>
+      <c r="D291" t="s">
+        <v>23</v>
+      </c>
+      <c r="E291">
+        <v>1</v>
+      </c>
+      <c r="F291" t="s">
+        <v>198</v>
+      </c>
+      <c r="H291" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I291" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J291" t="s">
+        <v>26</v>
+      </c>
+      <c r="K291" t="s">
+        <v>27</v>
+      </c>
+      <c r="M291" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="N291" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="292" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A292" s="34" t="s">
+        <v>738</v>
+      </c>
+      <c r="B292" t="s">
+        <v>198</v>
+      </c>
+      <c r="C292" t="s">
+        <v>702</v>
+      </c>
+      <c r="D292" t="s">
+        <v>23</v>
+      </c>
+      <c r="E292">
+        <v>1</v>
+      </c>
+      <c r="F292" t="s">
+        <v>198</v>
+      </c>
+      <c r="H292" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I292" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J292" t="s">
+        <v>26</v>
+      </c>
+      <c r="K292" t="s">
+        <v>27</v>
+      </c>
+      <c r="M292" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="N292" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="294" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A294" s="31" t="s">
+        <v>740</v>
+      </c>
+      <c r="B294" t="s">
+        <v>628</v>
+      </c>
+      <c r="C294" t="s">
+        <v>702</v>
+      </c>
+      <c r="D294" t="s">
+        <v>23</v>
+      </c>
+      <c r="E294">
+        <v>1</v>
+      </c>
+      <c r="F294" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="G294" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H294" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I294" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J294" t="s">
+        <v>26</v>
+      </c>
+      <c r="K294" t="s">
+        <v>27</v>
+      </c>
+      <c r="M294" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="N294" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA294" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB294" s="5"/>
+      <c r="AC294" s="5"/>
+      <c r="AD294" s="5"/>
+      <c r="AU294" s="17" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="295" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A295" s="31" t="s">
+        <v>741</v>
+      </c>
+      <c r="B295" t="s">
+        <v>628</v>
+      </c>
+      <c r="C295" t="s">
+        <v>702</v>
+      </c>
+      <c r="D295" t="s">
+        <v>23</v>
+      </c>
+      <c r="E295">
+        <v>1</v>
+      </c>
+      <c r="F295" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="G295" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H295" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I295" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J295" t="s">
+        <v>26</v>
+      </c>
+      <c r="K295" t="s">
+        <v>27</v>
+      </c>
+      <c r="M295" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="N295" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA295" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB295" s="5"/>
+      <c r="AC295" s="5"/>
+      <c r="AD295" s="5"/>
+      <c r="AU295" s="17" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="296" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A296" s="31" t="s">
+        <v>742</v>
+      </c>
+      <c r="B296" t="s">
+        <v>628</v>
+      </c>
+      <c r="C296" t="s">
+        <v>702</v>
+      </c>
+      <c r="D296" t="s">
+        <v>23</v>
+      </c>
+      <c r="E296">
+        <v>1</v>
+      </c>
+      <c r="F296" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="G296" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H296" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I296" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J296" t="s">
+        <v>26</v>
+      </c>
+      <c r="K296" t="s">
+        <v>27</v>
+      </c>
+      <c r="M296" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="N296" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA296" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB296" s="5"/>
+      <c r="AC296" s="5"/>
+      <c r="AD296" s="5"/>
+      <c r="AU296" s="17" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="297" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A297" s="31" t="s">
+        <v>743</v>
+      </c>
+      <c r="B297" t="s">
+        <v>628</v>
+      </c>
+      <c r="C297" t="s">
+        <v>702</v>
+      </c>
+      <c r="D297" t="s">
+        <v>23</v>
+      </c>
+      <c r="E297">
+        <v>1</v>
+      </c>
+      <c r="F297" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="G297" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H297" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I297" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J297" t="s">
+        <v>26</v>
+      </c>
+      <c r="K297" t="s">
+        <v>27</v>
+      </c>
+      <c r="M297" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="N297" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA297" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB297" s="5"/>
+      <c r="AC297" s="5"/>
+      <c r="AD297" s="5"/>
+      <c r="AU297" s="17" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="298" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A298" s="31" t="s">
+        <v>744</v>
+      </c>
+      <c r="B298" t="s">
+        <v>628</v>
+      </c>
+      <c r="C298" t="s">
+        <v>702</v>
+      </c>
+      <c r="D298" t="s">
+        <v>23</v>
+      </c>
+      <c r="E298">
+        <v>1</v>
+      </c>
+      <c r="F298" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="G298" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H298" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I298" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J298" t="s">
+        <v>26</v>
+      </c>
+      <c r="K298" t="s">
+        <v>27</v>
+      </c>
+      <c r="M298" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="N298" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA298" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB298" s="5"/>
+      <c r="AC298" s="5"/>
+      <c r="AD298" s="5"/>
+      <c r="AU298" s="17" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="299" spans="1:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="A299" s="31" t="s">
+        <v>745</v>
+      </c>
+      <c r="B299" t="s">
+        <v>628</v>
+      </c>
+      <c r="C299" t="s">
+        <v>702</v>
+      </c>
+      <c r="D299" t="s">
+        <v>23</v>
+      </c>
+      <c r="E299">
+        <v>1</v>
+      </c>
+      <c r="F299" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="G299" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H299" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I299" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J299" t="s">
+        <v>26</v>
+      </c>
+      <c r="K299" t="s">
+        <v>27</v>
+      </c>
+      <c r="M299" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="N299" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA299" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB299" s="5"/>
+      <c r="AC299" s="5"/>
+      <c r="AD299" s="5"/>
+      <c r="AU299" s="17" t="s">
+        <v>739</v>
       </c>
     </row>
   </sheetData>
@@ -16961,23 +18571,54 @@
     <hyperlink ref="H94" r:id="rId185"/>
     <hyperlink ref="H95" r:id="rId186"/>
     <hyperlink ref="H96" r:id="rId187"/>
-    <hyperlink ref="H243" r:id="rId188"/>
-    <hyperlink ref="H244" r:id="rId189"/>
-    <hyperlink ref="H245" r:id="rId190"/>
-    <hyperlink ref="H246" r:id="rId191"/>
-    <hyperlink ref="H247" r:id="rId192"/>
-    <hyperlink ref="H248" r:id="rId193"/>
-    <hyperlink ref="H249" r:id="rId194"/>
-    <hyperlink ref="H251" r:id="rId195"/>
-    <hyperlink ref="H252" r:id="rId196"/>
-    <hyperlink ref="H253" r:id="rId197"/>
-    <hyperlink ref="H254" r:id="rId198"/>
-    <hyperlink ref="H255" r:id="rId199"/>
-    <hyperlink ref="H256" r:id="rId200"/>
-    <hyperlink ref="H257" r:id="rId201"/>
+    <hyperlink ref="H246" r:id="rId188"/>
+    <hyperlink ref="H247" r:id="rId189"/>
+    <hyperlink ref="H248" r:id="rId190"/>
+    <hyperlink ref="H249" r:id="rId191"/>
+    <hyperlink ref="H250" r:id="rId192"/>
+    <hyperlink ref="H251" r:id="rId193"/>
+    <hyperlink ref="H252" r:id="rId194"/>
+    <hyperlink ref="H254" r:id="rId195"/>
+    <hyperlink ref="H255" r:id="rId196"/>
+    <hyperlink ref="H256" r:id="rId197"/>
+    <hyperlink ref="H257" r:id="rId198"/>
+    <hyperlink ref="H258" r:id="rId199"/>
+    <hyperlink ref="H259" r:id="rId200"/>
+    <hyperlink ref="H260" r:id="rId201"/>
+    <hyperlink ref="H263" r:id="rId202"/>
+    <hyperlink ref="H264" r:id="rId203"/>
+    <hyperlink ref="H265" r:id="rId204"/>
+    <hyperlink ref="H266" r:id="rId205"/>
+    <hyperlink ref="H267" r:id="rId206"/>
+    <hyperlink ref="H268" r:id="rId207"/>
+    <hyperlink ref="H269" r:id="rId208"/>
+    <hyperlink ref="H271" r:id="rId209"/>
+    <hyperlink ref="H272" r:id="rId210"/>
+    <hyperlink ref="H273" r:id="rId211"/>
+    <hyperlink ref="H274" r:id="rId212"/>
+    <hyperlink ref="H275" r:id="rId213"/>
+    <hyperlink ref="H276" r:id="rId214"/>
+    <hyperlink ref="H280" r:id="rId215"/>
+    <hyperlink ref="H281" r:id="rId216"/>
+    <hyperlink ref="H282" r:id="rId217"/>
+    <hyperlink ref="H283" r:id="rId218"/>
+    <hyperlink ref="H284" r:id="rId219"/>
+    <hyperlink ref="H285" r:id="rId220"/>
+    <hyperlink ref="H287" r:id="rId221"/>
+    <hyperlink ref="H288" r:id="rId222"/>
+    <hyperlink ref="H289" r:id="rId223"/>
+    <hyperlink ref="H290" r:id="rId224"/>
+    <hyperlink ref="H291" r:id="rId225"/>
+    <hyperlink ref="H292" r:id="rId226"/>
+    <hyperlink ref="H294" r:id="rId227"/>
+    <hyperlink ref="H295" r:id="rId228"/>
+    <hyperlink ref="H296" r:id="rId229"/>
+    <hyperlink ref="H297" r:id="rId230"/>
+    <hyperlink ref="H298" r:id="rId231"/>
+    <hyperlink ref="H299" r:id="rId232"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId202"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId233"/>
 </worksheet>
 </file>
 

</xml_diff>